<commit_message>
Added ChangePassword and FilterByCategory tests
</commit_message>
<xml_diff>
--- a/src/main/java/resources/xlsxFileWithTestData.xlsx
+++ b/src/main/java/resources/xlsxFileWithTestData.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="loginNegativeTests" sheetId="1" state="visible" r:id="rId3"/>
     <sheet name="loginValidCredentials" sheetId="2" state="visible" r:id="rId4"/>
     <sheet name="registerNegativeTests" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="changePasswordNegativeTests" sheetId="4" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="113">
   <si>
     <t xml:space="preserve">login</t>
   </si>
@@ -274,6 +275,226 @@
   </si>
   <si>
     <t xml:space="preserve">pass@1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">currentPassword</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newPassword</t>
+  </si>
+  <si>
+    <t xml:space="preserve">confirmNewPassword</t>
+  </si>
+  <si>
+    <t xml:space="preserve">111test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wrong current password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wrong current Password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This field is mandatory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">empty current Password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">123456t</t>
+  </si>
+  <si>
+    <t xml:space="preserve">only one criteria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@#$%&amp;@abc</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">only two criterias in </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve">newPassword</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Pass222</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">without symbol </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve">in newPassword</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">without capital letter </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve">in newPassword</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Te_1</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">less than min length </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve">in newPassword</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Тест123_test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cyrylic symbols in newPassword</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tes12_test</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">empty </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve"> newPassword</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">new password same as current</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">empty  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve">confirmNewPassword</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Test111@</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The passwords must match</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">wrong </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve">confirmNewPassword</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">confirmNewPassword same as current password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">all fields empty</t>
   </si>
 </sst>
 </file>
@@ -283,7 +504,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -367,6 +588,20 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -425,7 +660,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -492,6 +727,14 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1042,8 +1285,8 @@
   </sheetPr>
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1447,4 +1690,282 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Normalny"&amp;12&amp;KffffffPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F15"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="27.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="25.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="51.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="45.2"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F4" s="17"/>
+    </row>
+    <row r="5" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D15" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="Test@1234"/>
+    <hyperlink ref="B7" r:id="rId2" display="pass@1"/>
+    <hyperlink ref="C7" r:id="rId3" display="pass@1"/>
+    <hyperlink ref="B12" r:id="rId4" display="Test@1234"/>
+    <hyperlink ref="B13" r:id="rId5" display="Test@1234"/>
+    <hyperlink ref="B14" r:id="rId6" display="Test@1234"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normalny"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normalny"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>